<commit_message>
New god section added
</commit_message>
<xml_diff>
--- a/PetWebShop-pitanja.xlsx
+++ b/PetWebShop-pitanja.xlsx
@@ -285,12 +285,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -320,11 +326,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,19 +636,19 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G2" t="s">
@@ -649,19 +656,19 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
@@ -669,19 +676,19 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
     </row>
@@ -708,13 +715,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -739,24 +746,24 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>